<commit_message>
update show error label city
</commit_message>
<xml_diff>
--- a/Result_Sampling.xlsx
+++ b/Result_Sampling.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Phường Gia Định</t>
+          <t>Phường Tăng Nhơn Phú</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -484,7 +484,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Phường Dĩ An</t>
+          <t>Phường Chợ Lớn</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -502,7 +502,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Phường Cát Lái</t>
+          <t>Phường Tân Định</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -520,7 +520,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Phường Long Nguyên</t>
+          <t>Phường Linh Xuân</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -538,7 +538,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Phường An Khánh</t>
+          <t>Phường Tân Uyên</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -556,7 +556,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Phường Tây Thạnh</t>
+          <t>Phường Cầu Ông Lãnh</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -574,7 +574,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Phường Hòa Lợi</t>
+          <t>Phường Cầu Kiệu</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -592,7 +592,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Phường Bến Cát</t>
+          <t>Phường Tam Thắng</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -610,7 +610,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Phường Bình Đông</t>
+          <t>Phường Bình Lợi Trung</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -628,7 +628,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Xã An Thới Đông</t>
+          <t>Xã Kim Long</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Xã Long Hải</t>
+          <t>Xã Xuyên Mộc</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -664,7 +664,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Xã Vĩnh Lộc</t>
+          <t>Xã Ngãi Giao</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -682,7 +682,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Phường Hồng Hà</t>
+          <t>Phường Việt Hưng</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -700,7 +700,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Phường Láng</t>
+          <t>Phường Thượng Cát</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -718,7 +718,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Phường Vĩnh Tuy</t>
+          <t>Phường Lĩnh Nam</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -736,7 +736,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Phường Bồ Đề</t>
+          <t>Phường Yên Nghĩa</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -754,7 +754,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Phường Kiến Hưng</t>
+          <t>Phường Bồ Đề</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -772,7 +772,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Phường Tây Tựu</t>
+          <t>Phường Kiến Hưng</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -790,7 +790,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Phường Tây Hồ</t>
+          <t>Phường Ba Đình</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Xã Yên Xuân</t>
+          <t>Xã Liên Minh</t>
         </is>
       </c>
       <c r="D21" t="n">

</xml_diff>